<commit_message>
Excel is working now,
Note: An update of JAR files is required
</commit_message>
<xml_diff>
--- a/EngineTest2.xlsx
+++ b/EngineTest2.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Beta</t>
   </si>
@@ -104,13 +104,15 @@
   </si>
   <si>
     <t>Recipe-Sugar(gr)</t>
+  </si>
+  <si>
+    <t>Erdi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,26 +448,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.21875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.109375" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="16.88671875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="10" max="12" bestFit="true" customWidth="true" width="3.33203125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="6.21875" collapsed="true"/>
-    <col min="14" max="16" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -487,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -501,7 +503,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -515,7 +517,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -631,6 +633,38 @@
         <v>130</v>
       </c>
       <c r="J8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>130</v>
+      </c>
+      <c r="J9">
         <v>6</v>
       </c>
     </row>
@@ -641,15 +675,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -708,60 +742,60 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>100.0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="I2" t="n">
-        <v>130.0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.9750000000000001</v>
-      </c>
-      <c r="M2" t="n">
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2">
+        <v>130</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0.97500000000000009</v>
+      </c>
+      <c r="M2">
         <v>0.44999999999999996</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>2.86375</v>
       </c>
-      <c r="O2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="R2" t="n">
-        <v>0.0</v>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -779,4 +813,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Charts added. Small mistakes stay
</commit_message>
<xml_diff>
--- a/EngineTest2.xlsx
+++ b/EngineTest2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Beta</t>
   </si>
@@ -106,7 +106,64 @@
     <t>Recipe-Sugar(gr)</t>
   </si>
   <si>
-    <t>Erdi</t>
+    <t>shop0</t>
+  </si>
+  <si>
+    <t>shop1</t>
+  </si>
+  <si>
+    <t>shop2</t>
+  </si>
+  <si>
+    <t>shop3</t>
+  </si>
+  <si>
+    <t>shop4</t>
+  </si>
+  <si>
+    <t>shop5</t>
+  </si>
+  <si>
+    <t>shop6</t>
+  </si>
+  <si>
+    <t>shop7</t>
+  </si>
+  <si>
+    <t>shop8</t>
+  </si>
+  <si>
+    <t>shop9</t>
+  </si>
+  <si>
+    <t>shop10</t>
+  </si>
+  <si>
+    <t>shop11</t>
+  </si>
+  <si>
+    <t>shop12</t>
+  </si>
+  <si>
+    <t>shop13</t>
+  </si>
+  <si>
+    <t>shop14</t>
+  </si>
+  <si>
+    <t>shop15</t>
+  </si>
+  <si>
+    <t>shop16</t>
+  </si>
+  <si>
+    <t>shop17</t>
+  </si>
+  <si>
+    <t>shop18</t>
+  </si>
+  <si>
+    <t>shop19</t>
   </si>
 </sst>
 </file>
@@ -142,11 +199,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,7 +550,7 @@
         <v>50</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -506,7 +564,7 @@
         <v>40</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -520,7 +578,7 @@
         <v>30</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -606,22 +664,22 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B8">
         <v>100</v>
       </c>
       <c r="C8">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="D8">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="F8">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -638,22 +696,22 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>100</v>
       </c>
       <c r="C9">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="D9">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="F9">
-        <v>100</v>
+        <v>100000</v>
       </c>
       <c r="G9">
         <v>5</v>
@@ -665,6 +723,582 @@
         <v>130</v>
       </c>
       <c r="J9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>100000</v>
+      </c>
+      <c r="D10">
+        <v>100000</v>
+      </c>
+      <c r="E10">
+        <v>100000</v>
+      </c>
+      <c r="F10">
+        <v>100000</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>130</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>100000</v>
+      </c>
+      <c r="D11">
+        <v>100000</v>
+      </c>
+      <c r="E11">
+        <v>100000</v>
+      </c>
+      <c r="F11">
+        <v>100000</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
+      <c r="I11">
+        <v>130</v>
+      </c>
+      <c r="J11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>100000</v>
+      </c>
+      <c r="D12">
+        <v>100000</v>
+      </c>
+      <c r="E12">
+        <v>100000</v>
+      </c>
+      <c r="F12">
+        <v>100000</v>
+      </c>
+      <c r="G12">
+        <v>5</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>130</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>100000</v>
+      </c>
+      <c r="D13">
+        <v>100000</v>
+      </c>
+      <c r="E13">
+        <v>100000</v>
+      </c>
+      <c r="F13">
+        <v>100000</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>130</v>
+      </c>
+      <c r="J13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>100000</v>
+      </c>
+      <c r="D14">
+        <v>100000</v>
+      </c>
+      <c r="E14">
+        <v>100000</v>
+      </c>
+      <c r="F14">
+        <v>100000</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>130</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="C15">
+        <v>100000</v>
+      </c>
+      <c r="D15">
+        <v>100000</v>
+      </c>
+      <c r="E15">
+        <v>100000</v>
+      </c>
+      <c r="F15">
+        <v>100000</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>130</v>
+      </c>
+      <c r="J15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>100000</v>
+      </c>
+      <c r="D16">
+        <v>100000</v>
+      </c>
+      <c r="E16">
+        <v>100000</v>
+      </c>
+      <c r="F16">
+        <v>100000</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>10</v>
+      </c>
+      <c r="I16">
+        <v>130</v>
+      </c>
+      <c r="J16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <v>100</v>
+      </c>
+      <c r="C17">
+        <v>100000</v>
+      </c>
+      <c r="D17">
+        <v>100000</v>
+      </c>
+      <c r="E17">
+        <v>100000</v>
+      </c>
+      <c r="F17">
+        <v>100000</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>10</v>
+      </c>
+      <c r="I17">
+        <v>130</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <v>100</v>
+      </c>
+      <c r="C18">
+        <v>100000</v>
+      </c>
+      <c r="D18">
+        <v>100000</v>
+      </c>
+      <c r="E18">
+        <v>100000</v>
+      </c>
+      <c r="F18">
+        <v>100000</v>
+      </c>
+      <c r="G18" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>130</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>100000</v>
+      </c>
+      <c r="D19">
+        <v>100000</v>
+      </c>
+      <c r="E19">
+        <v>100000</v>
+      </c>
+      <c r="F19">
+        <v>100000</v>
+      </c>
+      <c r="G19" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19">
+        <v>130</v>
+      </c>
+      <c r="J19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <v>100</v>
+      </c>
+      <c r="C20">
+        <v>100000</v>
+      </c>
+      <c r="D20">
+        <v>100000</v>
+      </c>
+      <c r="E20">
+        <v>100000</v>
+      </c>
+      <c r="F20">
+        <v>100000</v>
+      </c>
+      <c r="G20" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="H20">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>130</v>
+      </c>
+      <c r="J20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21">
+        <v>100</v>
+      </c>
+      <c r="C21">
+        <v>100000</v>
+      </c>
+      <c r="D21">
+        <v>100000</v>
+      </c>
+      <c r="E21">
+        <v>100000</v>
+      </c>
+      <c r="F21">
+        <v>100000</v>
+      </c>
+      <c r="G21" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="H21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>130</v>
+      </c>
+      <c r="J21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22">
+        <v>100</v>
+      </c>
+      <c r="C22">
+        <v>100000</v>
+      </c>
+      <c r="D22">
+        <v>100000</v>
+      </c>
+      <c r="E22">
+        <v>100000</v>
+      </c>
+      <c r="F22">
+        <v>100000</v>
+      </c>
+      <c r="G22" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>130</v>
+      </c>
+      <c r="J22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <v>100</v>
+      </c>
+      <c r="C23">
+        <v>100000</v>
+      </c>
+      <c r="D23">
+        <v>100000</v>
+      </c>
+      <c r="E23">
+        <v>100000</v>
+      </c>
+      <c r="F23">
+        <v>100000</v>
+      </c>
+      <c r="G23">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>10</v>
+      </c>
+      <c r="I23">
+        <v>130</v>
+      </c>
+      <c r="J23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24">
+        <v>100</v>
+      </c>
+      <c r="C24">
+        <v>100000</v>
+      </c>
+      <c r="D24">
+        <v>100000</v>
+      </c>
+      <c r="E24">
+        <v>100000</v>
+      </c>
+      <c r="F24">
+        <v>100000</v>
+      </c>
+      <c r="G24">
+        <v>10</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+      <c r="I24">
+        <v>130</v>
+      </c>
+      <c r="J24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <v>100</v>
+      </c>
+      <c r="C25">
+        <v>100000</v>
+      </c>
+      <c r="D25">
+        <v>100000</v>
+      </c>
+      <c r="E25">
+        <v>100000</v>
+      </c>
+      <c r="F25">
+        <v>100000</v>
+      </c>
+      <c r="G25">
+        <v>10</v>
+      </c>
+      <c r="H25">
+        <v>10</v>
+      </c>
+      <c r="I25">
+        <v>130</v>
+      </c>
+      <c r="J25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <v>100</v>
+      </c>
+      <c r="C26">
+        <v>100000</v>
+      </c>
+      <c r="D26">
+        <v>100000</v>
+      </c>
+      <c r="E26">
+        <v>100000</v>
+      </c>
+      <c r="F26">
+        <v>100000</v>
+      </c>
+      <c r="G26">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <v>10</v>
+      </c>
+      <c r="I26">
+        <v>130</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27">
+        <v>100000</v>
+      </c>
+      <c r="D27">
+        <v>100000</v>
+      </c>
+      <c r="E27">
+        <v>100000</v>
+      </c>
+      <c r="F27">
+        <v>100000</v>
+      </c>
+      <c r="G27">
+        <v>10</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+      <c r="I27">
+        <v>130</v>
+      </c>
+      <c r="J27">
         <v>6</v>
       </c>
     </row>

</xml_diff>